<commit_message>
Add support for JS based map generator
</commit_message>
<xml_diff>
--- a/data/sample_employee_data.xlsx
+++ b/data/sample_employee_data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t>employee_id</t>
   </si>
@@ -35,22 +35,64 @@
     <t>office_longitude</t>
   </si>
   <si>
-    <t>Alice</t>
-  </si>
-  <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>Charlie</t>
-  </si>
-  <si>
-    <t>Deepak</t>
-  </si>
-  <si>
-    <t>Priya</t>
-  </si>
-  <si>
-    <t>Karthik</t>
+    <t>Employee_1</t>
+  </si>
+  <si>
+    <t>Employee_2</t>
+  </si>
+  <si>
+    <t>Employee_3</t>
+  </si>
+  <si>
+    <t>Employee_4</t>
+  </si>
+  <si>
+    <t>Employee_5</t>
+  </si>
+  <si>
+    <t>Employee_6</t>
+  </si>
+  <si>
+    <t>Employee_7</t>
+  </si>
+  <si>
+    <t>Employee_8</t>
+  </si>
+  <si>
+    <t>Employee_9</t>
+  </si>
+  <si>
+    <t>Employee_10</t>
+  </si>
+  <si>
+    <t>Employee_11</t>
+  </si>
+  <si>
+    <t>Employee_12</t>
+  </si>
+  <si>
+    <t>Employee_13</t>
+  </si>
+  <si>
+    <t>Employee_14</t>
+  </si>
+  <si>
+    <t>Employee_15</t>
+  </si>
+  <si>
+    <t>Employee_16</t>
+  </si>
+  <si>
+    <t>Employee_17</t>
+  </si>
+  <si>
+    <t>Employee_18</t>
+  </si>
+  <si>
+    <t>Employee_19</t>
+  </si>
+  <si>
+    <t>Employee_20</t>
   </si>
 </sst>
 </file>
@@ -408,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -436,62 +478,302 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2">
-        <v>37.7749</v>
+        <v>28.38819313027635</v>
       </c>
       <c r="D2">
-        <v>-122.4194</v>
+        <v>-106.6074184746828</v>
       </c>
       <c r="E2">
-        <v>37.7749</v>
+        <v>28.88056487831371</v>
       </c>
       <c r="F2">
-        <v>-122.4194</v>
+        <v>-106.2588411840927</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>102</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3">
-        <v>34.0522</v>
+        <v>29.1412690214571</v>
       </c>
       <c r="D3">
-        <v>-118.2437</v>
+        <v>-105.8845923383558</v>
       </c>
       <c r="E3">
-        <v>40.7128</v>
+        <v>28.88056487831371</v>
       </c>
       <c r="F3">
-        <v>-74.006</v>
+        <v>-106.2588411840927</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>103</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4">
-        <v>40.7128</v>
+        <v>29.33403596141372</v>
       </c>
       <c r="D4">
-        <v>-74.006</v>
+        <v>-106.5126085241606</v>
       </c>
       <c r="E4">
-        <v>34.0522</v>
+        <v>28.88056487831371</v>
       </c>
       <c r="F4">
-        <v>-118.2437</v>
+        <v>-106.2588411840927</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>28.76904351201771</v>
+      </c>
+      <c r="D5">
+        <v>-105.8512008029425</v>
+      </c>
+      <c r="E5">
+        <v>28.88056487831371</v>
+      </c>
+      <c r="F5">
+        <v>-106.2588411840927</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>29.35371651305762</v>
+      </c>
+      <c r="D6">
+        <v>-106.3661007722006</v>
+      </c>
+      <c r="E6">
+        <v>28.88056487831371</v>
+      </c>
+      <c r="F6">
+        <v>-106.2588411840927</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>41.92919387720103</v>
+      </c>
+      <c r="D7">
+        <v>-97.34409830136389</v>
+      </c>
+      <c r="E7">
+        <v>42.14550328523458</v>
+      </c>
+      <c r="F7">
+        <v>-97.62862974982434</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>42.14495047403216</v>
+      </c>
+      <c r="D8">
+        <v>-98.06567273365452</v>
+      </c>
+      <c r="E8">
+        <v>42.14550328523458</v>
+      </c>
+      <c r="F8">
+        <v>-97.62862974982434</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>42.26054203379384</v>
+      </c>
+      <c r="D9">
+        <v>-97.32827576251987</v>
+      </c>
+      <c r="E9">
+        <v>42.14550328523458</v>
+      </c>
+      <c r="F9">
+        <v>-97.62862974982434</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>41.9195817108412</v>
+      </c>
+      <c r="D10">
+        <v>-98.10187844626958</v>
+      </c>
+      <c r="E10">
+        <v>42.14550328523458</v>
+      </c>
+      <c r="F10">
+        <v>-97.62862974982434</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>41.72017968958709</v>
+      </c>
+      <c r="D11">
+        <v>-97.99903571399425</v>
+      </c>
+      <c r="E11">
+        <v>42.14550328523458</v>
+      </c>
+      <c r="F11">
+        <v>-97.62862974982434</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>38.37424919151829</v>
+      </c>
+      <c r="D12">
+        <v>-100.6826195356586</v>
+      </c>
+      <c r="E12">
+        <v>37.91914745309903</v>
+      </c>
+      <c r="F12">
+        <v>-100.2541194271461</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>37.72527774484379</v>
+      </c>
+      <c r="D13">
+        <v>-100.512675324642</v>
+      </c>
+      <c r="E13">
+        <v>37.91914745309903</v>
+      </c>
+      <c r="F13">
+        <v>-100.2541194271461</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>37.74701525398464</v>
+      </c>
+      <c r="D14">
+        <v>-99.78824212183413</v>
+      </c>
+      <c r="E14">
+        <v>37.91914745309903</v>
+      </c>
+      <c r="F14">
+        <v>-100.2541194271461</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <v>37.66515129855738</v>
+      </c>
+      <c r="D15">
+        <v>-99.88545225556149</v>
+      </c>
+      <c r="E15">
+        <v>37.91914745309903</v>
+      </c>
+      <c r="F15">
+        <v>-100.2541194271461</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>38.32176325719586</v>
+      </c>
+      <c r="D16">
+        <v>-100.2947423437324</v>
+      </c>
+      <c r="E16">
+        <v>37.91914745309903</v>
+      </c>
+      <c r="F16">
+        <v>-100.2541194271461</v>
       </c>
     </row>
   </sheetData>
@@ -501,7 +783,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -529,62 +811,402 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>201</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>28.7041</v>
+        <v>16.43095972333562</v>
       </c>
       <c r="D2">
-        <v>77.10250000000001</v>
+        <v>86.46361764823395</v>
       </c>
       <c r="E2">
-        <v>28.7041</v>
+        <v>16.06354539373788</v>
       </c>
       <c r="F2">
-        <v>77.10250000000001</v>
+        <v>86.65614996209709</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>202</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>19.076</v>
+        <v>16.51636122365941</v>
       </c>
       <c r="D3">
-        <v>72.8777</v>
+        <v>86.85039665213945</v>
       </c>
       <c r="E3">
-        <v>19.076</v>
+        <v>16.06354539373788</v>
       </c>
       <c r="F3">
-        <v>72.8777</v>
+        <v>86.65614996209709</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>203</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>16.11167689724853</v>
+      </c>
+      <c r="D4">
+        <v>87.04338288506732</v>
+      </c>
+      <c r="E4">
+        <v>16.06354539373788</v>
+      </c>
+      <c r="F4">
+        <v>86.65614996209709</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>16.1974904042192</v>
+      </c>
+      <c r="D5">
+        <v>87.12674817498186</v>
+      </c>
+      <c r="E5">
+        <v>16.06354539373788</v>
+      </c>
+      <c r="F5">
+        <v>86.65614996209709</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>15.61758000039879</v>
+      </c>
+      <c r="D6">
+        <v>86.21218181375453</v>
+      </c>
+      <c r="E6">
+        <v>16.06354539373788</v>
+      </c>
+      <c r="F6">
+        <v>86.65614996209709</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C4">
-        <v>13.0827</v>
-      </c>
-      <c r="D4">
-        <v>80.27070000000001</v>
-      </c>
-      <c r="E4">
-        <v>13.0827</v>
-      </c>
-      <c r="F4">
-        <v>80.27070000000001</v>
+      <c r="C7">
+        <v>26.23902397444644</v>
+      </c>
+      <c r="D7">
+        <v>84.8962715331638</v>
+      </c>
+      <c r="E7">
+        <v>26.18940097694169</v>
+      </c>
+      <c r="F7">
+        <v>84.56886789228395</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>26.11369387290055</v>
+      </c>
+      <c r="D8">
+        <v>84.4236433105559</v>
+      </c>
+      <c r="E8">
+        <v>26.18940097694169</v>
+      </c>
+      <c r="F8">
+        <v>84.56886789228395</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>25.92053186072961</v>
+      </c>
+      <c r="D9">
+        <v>84.31520141966945</v>
+      </c>
+      <c r="E9">
+        <v>26.18940097694169</v>
+      </c>
+      <c r="F9">
+        <v>84.56886789228395</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>26.18485850192749</v>
+      </c>
+      <c r="D10">
+        <v>84.14365542892563</v>
+      </c>
+      <c r="E10">
+        <v>26.18940097694169</v>
+      </c>
+      <c r="F10">
+        <v>84.56886789228395</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>26.6718206128723</v>
+      </c>
+      <c r="D11">
+        <v>84.27835942315853</v>
+      </c>
+      <c r="E11">
+        <v>26.18940097694169</v>
+      </c>
+      <c r="F11">
+        <v>84.56886789228395</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>22.56922971056579</v>
+      </c>
+      <c r="D12">
+        <v>88.14506410447565</v>
+      </c>
+      <c r="E12">
+        <v>22.7084536475339</v>
+      </c>
+      <c r="F12">
+        <v>87.79338757895121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>22.36911905649291</v>
+      </c>
+      <c r="D13">
+        <v>87.66985008029674</v>
+      </c>
+      <c r="E13">
+        <v>22.7084536475339</v>
+      </c>
+      <c r="F13">
+        <v>87.79338757895121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>22.29474225518964</v>
+      </c>
+      <c r="D14">
+        <v>87.73837786710999</v>
+      </c>
+      <c r="E14">
+        <v>22.7084536475339</v>
+      </c>
+      <c r="F14">
+        <v>87.79338757895121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <v>22.41219223215229</v>
+      </c>
+      <c r="D15">
+        <v>87.74994984391624</v>
+      </c>
+      <c r="E15">
+        <v>22.7084536475339</v>
+      </c>
+      <c r="F15">
+        <v>87.79338757895121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>22.34444070012497</v>
+      </c>
+      <c r="D16">
+        <v>87.61691259733716</v>
+      </c>
+      <c r="E16">
+        <v>22.7084536475339</v>
+      </c>
+      <c r="F16">
+        <v>87.79338757895121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>16.96023529004102</v>
+      </c>
+      <c r="D17">
+        <v>86.63037291093129</v>
+      </c>
+      <c r="E17">
+        <v>16.78927055243165</v>
+      </c>
+      <c r="F17">
+        <v>86.25880985887343</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>16.95058852625284</v>
+      </c>
+      <c r="D18">
+        <v>86.54420326976596</v>
+      </c>
+      <c r="E18">
+        <v>16.78927055243165</v>
+      </c>
+      <c r="F18">
+        <v>86.25880985887343</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19">
+        <v>16.83075184160061</v>
+      </c>
+      <c r="D19">
+        <v>85.99642583037293</v>
+      </c>
+      <c r="E19">
+        <v>16.78927055243165</v>
+      </c>
+      <c r="F19">
+        <v>86.25880985887343</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20">
+        <v>16.96163117117006</v>
+      </c>
+      <c r="D20">
+        <v>86.15327467696248</v>
+      </c>
+      <c r="E20">
+        <v>16.78927055243165</v>
+      </c>
+      <c r="F20">
+        <v>86.25880985887343</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21">
+        <v>17.23108499564752</v>
+      </c>
+      <c r="D21">
+        <v>85.79907793024336</v>
+      </c>
+      <c r="E21">
+        <v>16.78927055243165</v>
+      </c>
+      <c r="F21">
+        <v>86.25880985887343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>